<commit_message>
Expense Cycle Closed v2
</commit_message>
<xml_diff>
--- a/public/expenses/item_template.xlsx
+++ b/public/expenses/item_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SkillRev\Schoollms\skillrev\storage\app\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5C3B5F-7F42-4C27-811D-26DBC7CD792A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194B6DF6-7C52-4C26-B0EF-901507A2F9C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7DBF81E2-0B35-422B-938A-166055E16A3C}"/>
   </bookViews>
@@ -27,10 +27,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Item</t>
+    <t>item</t>
   </si>
   <si>
-    <t>quantity</t>
+    <t>quantity_measure</t>
   </si>
 </sst>
 </file>
@@ -415,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{524E6B66-B0A4-4873-B989-AE87BCC4C9AF}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -438,11 +438,10 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="C1" s="3"/>
       <c r="F1" s="2"/>
     </row>
+    <row r="5" spans="1:6" ht="4.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>